<commit_message>
modifie excel with added channel and implement first slide 2 logic
</commit_message>
<xml_diff>
--- a/data_modified.xlsx
+++ b/data_modified.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\valwur0b\Desktop\mindsphere\GCP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\valen\Desktop\Programmieren\GCP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81BBE303-95EC-45C0-8BE2-1EAE8997A1D7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D24AF20C-E5EF-4E84-BAF8-8C8F7C93F279}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25320" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="7">
   <si>
     <t>Time</t>
   </si>
@@ -52,6 +52,9 @@
   </si>
   <si>
     <t>CYW</t>
+  </si>
+  <si>
+    <t>PUE</t>
   </si>
 </sst>
 </file>
@@ -91,7 +94,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -369,15 +372,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E34"/>
+  <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -394,7 +397,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>17</v>
       </c>
@@ -411,7 +414,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>17</v>
       </c>
@@ -428,7 +431,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>17</v>
       </c>
@@ -445,7 +448,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>17</v>
       </c>
@@ -462,7 +465,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>17</v>
       </c>
@@ -479,7 +482,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>17</v>
       </c>
@@ -496,7 +499,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>17</v>
       </c>
@@ -513,7 +516,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>17</v>
       </c>
@@ -530,7 +533,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>17</v>
       </c>
@@ -547,7 +550,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>17</v>
       </c>
@@ -564,7 +567,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>17</v>
       </c>
@@ -581,7 +584,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>17</v>
       </c>
@@ -598,7 +601,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>17</v>
       </c>
@@ -615,7 +618,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>17</v>
       </c>
@@ -632,7 +635,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>17</v>
       </c>
@@ -649,7 +652,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>17</v>
       </c>
@@ -657,16 +660,16 @@
         <v>16</v>
       </c>
       <c r="C17" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D17">
         <v>1</v>
       </c>
       <c r="E17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
@@ -674,7 +677,7 @@
         <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D18">
         <v>2</v>
@@ -683,7 +686,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>17</v>
       </c>
@@ -691,16 +694,16 @@
         <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D19">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>17</v>
       </c>
@@ -717,7 +720,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>17</v>
       </c>
@@ -734,7 +737,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>17</v>
       </c>
@@ -751,7 +754,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>17</v>
       </c>
@@ -768,7 +771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>17</v>
       </c>
@@ -785,7 +788,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>17</v>
       </c>
@@ -802,7 +805,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>17</v>
       </c>
@@ -819,7 +822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>17</v>
       </c>
@@ -833,10 +836,10 @@
         <v>2</v>
       </c>
       <c r="E27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>17</v>
       </c>
@@ -853,7 +856,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>17</v>
       </c>
@@ -870,7 +873,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>17</v>
       </c>
@@ -887,7 +890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>17</v>
       </c>
@@ -904,7 +907,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>17</v>
       </c>
@@ -921,7 +924,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>17</v>
       </c>
@@ -935,10 +938,10 @@
         <v>2</v>
       </c>
       <c r="E33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>17</v>
       </c>
@@ -952,6 +955,57 @@
         <v>3</v>
       </c>
       <c r="E34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A35">
+        <v>17</v>
+      </c>
+      <c r="B35">
+        <v>34</v>
+      </c>
+      <c r="C35" t="s">
+        <v>5</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A36">
+        <v>17</v>
+      </c>
+      <c r="B36">
+        <v>35</v>
+      </c>
+      <c r="C36" t="s">
+        <v>5</v>
+      </c>
+      <c r="D36">
+        <v>2</v>
+      </c>
+      <c r="E36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A37">
+        <v>17</v>
+      </c>
+      <c r="B37">
+        <v>36</v>
+      </c>
+      <c r="C37" t="s">
+        <v>5</v>
+      </c>
+      <c r="D37">
+        <v>3</v>
+      </c>
+      <c r="E37">
         <v>1</v>
       </c>
     </row>

</xml_diff>